<commit_message>
added CapStatements,  fixed subscription interaction diagrams, QA, package-list.json
</commit_message>
<xml_diff>
--- a/source/resources/source-data/alert-intermediary-client.xlsx
+++ b/source/resources/source-data/alert-intermediary-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\source\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C73014C-A383-4210-A139-2BCAD4E15955}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D44CD-7CA5-42F0-B136-17721FA03EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -360,9 +360,6 @@
     <t>doc_DiagnosticReport</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/CapabilityStatement/hl7.fhir.us.davinci-alerts-0.0.0</t>
-  </si>
-  <si>
     <t>Communication</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   <si>
     <t>1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
 1. For security considerations specific to this guide refer to the  [Security](security.html) page for requirements and recommendations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts-0.0.0</t>
   </si>
 </sst>
 </file>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -919,7 +919,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1">
@@ -927,7 +927,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -935,7 +935,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -943,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="351.75" customHeight="1">
@@ -951,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="103.5" customHeight="1">
@@ -959,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -993,10 +993,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -1039,16 +1039,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="2" spans="1:23" ht="15.75" thickTop="1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
@@ -1407,13 +1407,13 @@
         <v>79</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -2002,25 +2002,25 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="90">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -2028,7 +2028,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -2711,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
add alert bundle profile, notify operation, updated cap statements
</commit_message>
<xml_diff>
--- a/source/resources/source-data/alert-intermediary-client.xlsx
+++ b/source/resources/source-data/alert-intermediary-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\source\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D44CD-7CA5-42F0-B136-17721FA03EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85FB37-C58F-4B4E-95B9-E91E85F89E1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="124">
   <si>
     <t>Element</t>
   </si>
@@ -372,18 +372,12 @@
     <t>Coverage</t>
   </si>
   <si>
-    <t>Subscription</t>
-  </si>
-  <si>
     <t>conf_Communication</t>
   </si>
   <si>
     <t>conf_Coverage</t>
   </si>
   <si>
-    <t>conf_Subscription</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core-3.0.0</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
   </si>
   <si>
     <t>doc</t>
-  </si>
-  <si>
-    <t>Whether as a direct push based transaction or via subscription notification, a common  `transaction`  type “Alert Bundle” is the FHIR object that is exchanged between the Da Vinci Alert Actors.</t>
   </si>
   <si>
     <t>alert-intermediary-client</t>
@@ -427,14 +418,45 @@
 1. For security considerations specific to this guide refer to the  [Security](security.html) page for requirements and recommendations.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts-0.0.0</t>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/alerts-bundle</t>
+  </si>
+  <si>
+    <t>Da Vinci Alerts Bundle Profile</t>
+  </si>
+  <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
+  </si>
+  <si>
+    <t>HRex Coverage Profile</t>
+  </si>
+  <si>
+    <t>notify</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/OperationDefinition/notify</t>
+  </si>
+  <si>
+    <t>conf_Bundle</t>
+  </si>
+  <si>
+    <t>A common  `transaction`  type “Alert Bundle” is the FHIR object that is exchanged between the Da Vinci Alert Actors.</t>
+  </si>
+  <si>
+    <t>A client **SHOULD** be capable of processing and responding to a $notify operation.
+`GET [base]/DocumentReference/$docref?patient=[id]`</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts-0.1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +527,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -551,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -579,6 +607,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -897,7 +926,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -919,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1">
@@ -927,7 +956,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -935,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -943,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="351.75" customHeight="1">
@@ -951,7 +980,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="103.5" customHeight="1">
@@ -959,7 +988,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -993,10 +1022,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -1011,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1053,13 +1082,33 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
@@ -1141,7 +1190,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1259,7 +1308,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
@@ -1293,7 +1342,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1321,10 +1370,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="E4" s="2"/>
@@ -1339,8 +1400,8 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R12" sqref="R12"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1407,13 +1468,13 @@
         <v>79</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1985,7 +2046,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2002,25 +2063,25 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="103.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
@@ -2028,7 +2089,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -2036,7 +2097,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated notify operation to add endpoint information
</commit_message>
<xml_diff>
--- a/source/resources/source-data/alert-intermediary-client.xlsx
+++ b/source/resources/source-data/alert-intermediary-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\source\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85FB37-C58F-4B4E-95B9-E91E85F89E1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DED467D-AED1-48B3-9CD4-281A65BEC114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="129">
   <si>
     <t>Element</t>
   </si>
@@ -450,6 +450,21 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts-0.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/alerts-endpoint</t>
+  </si>
+  <si>
+    <t>Da Vinci Alerts Endpoint Profile</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>SHALL</t>
+  </si>
+  <si>
+    <t>conf_Endpoint</t>
   </si>
 </sst>
 </file>
@@ -925,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1041,7 +1056,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1073,8 +1088,8 @@
       <c r="B2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" t="s">
-        <v>54</v>
+      <c r="C2" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="D2" t="s">
         <v>95</v>
@@ -1089,7 +1104,7 @@
         <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>115</v>
@@ -1112,6 +1127,18 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
@@ -1190,7 +1217,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1320,8 +1347,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5"/>
+    <row r="5" spans="1:23" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="R5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="20:23" ht="18">
       <c r="T36" s="7"/>
@@ -1397,11 +1436,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W9" sqref="W9"/>
+      <selection pane="topRight" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1412,7 +1451,7 @@
     <col min="4" max="4" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1476,8 +1515,11 @@
       <c r="U1" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1536,10 +1578,13 @@
         <v>26</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>26</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1600,8 +1645,11 @@
       <c r="U3" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1662,8 +1710,11 @@
       <c r="U4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1724,8 +1775,11 @@
       <c r="U5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1786,8 +1840,11 @@
       <c r="U6" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1848,8 +1905,11 @@
       <c r="U7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1908,10 +1968,13 @@
         <v>26</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+        <v>26</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1972,8 +2035,11 @@
       <c r="U9" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2032,6 +2098,9 @@
         <v>26</v>
       </c>
       <c r="U10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2045,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418CE29-40DC-476E-89CD-A42CEC26847E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>